<commit_message>
fix: minor bur important changes in the task. such as adding new TR control code. New event data added as well.
</commit_message>
<xml_diff>
--- a/events/sub-t_task-sentences_events.xlsx
+++ b/events/sub-t_task-sentences_events.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1287" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1403" uniqueCount="8">
   <si>
     <t>TR</t>
   </si>
@@ -117,13 +117,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>1.9997708999999304</v>
+        <v>2.0005650000000514</v>
       </c>
       <c r="C2" s="0">
-        <v>2179.7928230000002</v>
+        <v>1998.0601435999999</v>
       </c>
       <c r="D2" s="0">
-        <v>2181.7945764000001</v>
+        <v>2000.0619563</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>5</v>
@@ -134,13 +134,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>3.9987768999999389</v>
+        <v>4.0000984000000699</v>
       </c>
       <c r="C3" s="0">
-        <v>2179.7931005</v>
+        <v>1998.0604370999999</v>
       </c>
       <c r="D3" s="0">
-        <v>2183.7935824000001</v>
+        <v>2002.0614897</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>5</v>
@@ -151,13 +151,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>5.9986363999996684</v>
+        <v>5.9994818000000123</v>
       </c>
       <c r="C4" s="0">
-        <v>2179.7931009999998</v>
+        <v>1998.0604378999999</v>
       </c>
       <c r="D4" s="0">
-        <v>2185.7934418999998</v>
+        <v>2004.0608731</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>5</v>
@@ -168,13 +168,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>7.9986332999997103</v>
+        <v>7.9998361000000386</v>
       </c>
       <c r="C5" s="0">
-        <v>2179.7931006999997</v>
+        <v>1998.0604373000001</v>
       </c>
       <c r="D5" s="0">
-        <v>2187.7934387999999</v>
+        <v>2006.0612274</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>5</v>
@@ -185,13 +185,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>9.9987468999997873</v>
+        <v>9.9995304000001397</v>
       </c>
       <c r="C6" s="0">
-        <v>2179.7931006999997</v>
+        <v>1998.0604390000001</v>
       </c>
       <c r="D6" s="0">
-        <v>2189.7935524</v>
+        <v>2008.0609217000001</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>5</v>
@@ -202,13 +202,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>11.998674799999662</v>
+        <v>11.99948940000013</v>
       </c>
       <c r="C7" s="0">
-        <v>2179.7931014999999</v>
+        <v>1998.0604389</v>
       </c>
       <c r="D7" s="0">
-        <v>2191.7934802999998</v>
+        <v>2010.0608807000001</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>5</v>
@@ -219,13 +219,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>13.998685399999886</v>
+        <v>13.999432200000001</v>
       </c>
       <c r="C8" s="0">
-        <v>2179.7931013000002</v>
+        <v>1998.0604394</v>
       </c>
       <c r="D8" s="0">
-        <v>2193.7934909000001</v>
+        <v>2012.0608235</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>5</v>
@@ -236,13 +236,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>15.998733099999754</v>
+        <v>15.999476899999991</v>
       </c>
       <c r="C9" s="0">
-        <v>2179.7931008999999</v>
+        <v>1998.0604346</v>
       </c>
       <c r="D9" s="0">
-        <v>2195.7935385999999</v>
+        <v>2014.0608682</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>5</v>
@@ -253,13 +253,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0">
-        <v>17.99869979999994</v>
+        <v>17.999506399999973</v>
       </c>
       <c r="C10" s="0">
-        <v>2179.7931011999999</v>
+        <v>1998.0604386</v>
       </c>
       <c r="D10" s="0">
-        <v>2197.7935053000001</v>
+        <v>2016.0608976999999</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>5</v>
@@ -270,13 +270,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0">
-        <v>19.99865490000002</v>
+        <v>19.999389999999948</v>
       </c>
       <c r="C11" s="0">
-        <v>2179.7931011000001</v>
+        <v>1998.0604395</v>
       </c>
       <c r="D11" s="0">
-        <v>2199.7934604000002</v>
+        <v>2018.0607812999999</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>5</v>
@@ -287,13 +287,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0">
-        <v>21.998739199999818</v>
+        <v>21.999400599999944</v>
       </c>
       <c r="C12" s="0">
-        <v>2179.7931011000001</v>
+        <v>1998.0604394</v>
       </c>
       <c r="D12" s="0">
-        <v>2201.7935447</v>
+        <v>2020.0607918999999</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>5</v>
@@ -304,13 +304,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0">
-        <v>23.99887119999994</v>
+        <v>23.999452100000099</v>
       </c>
       <c r="C13" s="0">
-        <v>2179.7930992000001</v>
+        <v>1998.0604393000001</v>
       </c>
       <c r="D13" s="0">
-        <v>2203.7936767000001</v>
+        <v>2022.0608434000001</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>5</v>
@@ -321,13 +321,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0">
-        <v>25.998657999999978</v>
+        <v>25.999831900000117</v>
       </c>
       <c r="C14" s="0">
-        <v>2179.7931012000004</v>
+        <v>1998.0604369</v>
       </c>
       <c r="D14" s="0">
-        <v>2205.7934635000001</v>
+        <v>2024.0612232000001</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>5</v>
@@ -338,13 +338,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0">
-        <v>27.998698299999887</v>
+        <v>27.999381900000117</v>
       </c>
       <c r="C15" s="0">
-        <v>2179.7931008999999</v>
+        <v>1998.0604393000001</v>
       </c>
       <c r="D15" s="0">
-        <v>2207.7935038000001</v>
+        <v>2026.0607732000001</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>5</v>
@@ -355,13 +355,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0">
-        <v>29.998632299999827</v>
+        <v>30.000027199999977</v>
       </c>
       <c r="C16" s="0">
-        <v>2179.7931008999999</v>
+        <v>1998.0604392</v>
       </c>
       <c r="D16" s="0">
-        <v>2209.7934378</v>
+        <v>2028.0614184999999</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>5</v>
@@ -372,13 +372,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0">
-        <v>31.998647399999754</v>
+        <v>31.999517400000059</v>
       </c>
       <c r="C17" s="0">
-        <v>2179.7931009999998</v>
+        <v>1998.0604390000001</v>
       </c>
       <c r="D17" s="0">
-        <v>2211.7934528999999</v>
+        <v>2030.0609087</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>5</v>
@@ -386,88 +386,78 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B18" s="0">
-        <v>33.999204199999895</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0">
-        <v>2179.7930707999999</v>
+        <v>0</v>
       </c>
       <c r="D18" s="0">
-        <v>2213.7940097000001</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>6</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E18" s="0"/>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B19" s="0">
-        <v>35.998889199999667</v>
+        <v>0</v>
       </c>
       <c r="C19" s="0">
-        <v>2179.7930549999996</v>
+        <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>2215.7936946999998</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>6</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E19" s="0"/>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B20" s="0">
-        <v>37.998665899999651</v>
+        <v>0</v>
       </c>
       <c r="C20" s="0">
-        <v>2179.7930766999998</v>
+        <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>2217.7934713999998</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>6</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E20" s="0"/>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B21" s="0">
-        <v>39.998626699999932</v>
+        <v>0</v>
       </c>
       <c r="C21" s="0">
-        <v>2179.7930812</v>
+        <v>0</v>
       </c>
       <c r="D21" s="0">
-        <v>2219.7934322000001</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>6</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E21" s="0"/>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22" s="0">
-        <v>41.999167299999954</v>
+        <v>0</v>
       </c>
       <c r="C22" s="0">
-        <v>2179.7929998</v>
+        <v>0</v>
       </c>
       <c r="D22" s="0">
-        <v>2221.7939728000001</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>6</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E22" s="0"/>
     </row>
     <row r="23">
       <c r="A23" s="0">

</xml_diff>

<commit_message>
data files and complete task
</commit_message>
<xml_diff>
--- a/events/sub-t_task-sentences_events.xlsx
+++ b/events/sub-t_task-sentences_events.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1403" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2240" uniqueCount="8">
   <si>
     <t>TR</t>
   </si>
@@ -117,13 +117,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>2.0005650000000514</v>
+        <v>1.9996210999961477</v>
       </c>
       <c r="C2" s="0">
-        <v>1998.0601435999999</v>
+        <v>120031.5436572</v>
       </c>
       <c r="D2" s="0">
-        <v>2000.0619563</v>
+        <v>120033.5439247</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>5</v>
@@ -134,13 +134,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>4.0000984000000699</v>
+        <v>3.9999316999892471</v>
       </c>
       <c r="C3" s="0">
-        <v>1998.0604370999999</v>
+        <v>120031.54365409999</v>
       </c>
       <c r="D3" s="0">
-        <v>2002.0614897</v>
+        <v>120035.5442353</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>5</v>
@@ -151,13 +151,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>5.9994818000000123</v>
+        <v>5.9996259999898029</v>
       </c>
       <c r="C4" s="0">
-        <v>1998.0604378999999</v>
+        <v>120031.543657</v>
       </c>
       <c r="D4" s="0">
-        <v>2004.0608731</v>
+        <v>120037.5439296</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>5</v>
@@ -168,13 +168,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>7.9998361000000386</v>
+        <v>7.9996422999975039</v>
       </c>
       <c r="C5" s="0">
-        <v>1998.0604373000001</v>
+        <v>120031.5436572</v>
       </c>
       <c r="D5" s="0">
-        <v>2006.0612274</v>
+        <v>120039.5439459</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>5</v>
@@ -185,13 +185,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>9.9995304000001397</v>
+        <v>9.9996038999961456</v>
       </c>
       <c r="C6" s="0">
-        <v>1998.0604390000001</v>
+        <v>120031.5436569</v>
       </c>
       <c r="D6" s="0">
-        <v>2008.0609217000001</v>
+        <v>120041.5439075</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>5</v>
@@ -202,13 +202,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>11.99948940000013</v>
+        <v>11.999655699997675</v>
       </c>
       <c r="C7" s="0">
-        <v>1998.0604389</v>
+        <v>120031.5436569</v>
       </c>
       <c r="D7" s="0">
-        <v>2010.0608807000001</v>
+        <v>120043.5439593</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>5</v>
@@ -219,13 +219,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>13.999432200000001</v>
+        <v>13.999594499997329</v>
       </c>
       <c r="C8" s="0">
-        <v>1998.0604394</v>
+        <v>120031.5436572</v>
       </c>
       <c r="D8" s="0">
-        <v>2012.0608235</v>
+        <v>120045.5438981</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>5</v>
@@ -236,13 +236,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>15.999476899999991</v>
+        <v>15.99994069999957</v>
       </c>
       <c r="C9" s="0">
-        <v>1998.0604346</v>
+        <v>120031.5436571</v>
       </c>
       <c r="D9" s="0">
-        <v>2014.0608682</v>
+        <v>120047.54424430001</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>5</v>
@@ -253,13 +253,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0">
-        <v>17.999506399999973</v>
+        <v>17.999661099995137</v>
       </c>
       <c r="C10" s="0">
-        <v>1998.0604386</v>
+        <v>120031.5436566</v>
       </c>
       <c r="D10" s="0">
-        <v>2016.0608976999999</v>
+        <v>120049.5439647</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>5</v>
@@ -270,13 +270,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0">
-        <v>19.999389999999948</v>
+        <v>19.999602699987008</v>
       </c>
       <c r="C11" s="0">
-        <v>1998.0604395</v>
+        <v>120031.54365749999</v>
       </c>
       <c r="D11" s="0">
-        <v>2018.0607812999999</v>
+        <v>120051.54390629999</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>5</v>
@@ -287,13 +287,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0">
-        <v>21.999400599999944</v>
+        <v>21.99964199999522</v>
       </c>
       <c r="C12" s="0">
-        <v>1998.0604394</v>
+        <v>120031.5436569</v>
       </c>
       <c r="D12" s="0">
-        <v>2020.0607918999999</v>
+        <v>120053.5439456</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>5</v>
@@ -304,13 +304,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0">
-        <v>23.999452100000099</v>
+        <v>23.999679399988963</v>
       </c>
       <c r="C13" s="0">
-        <v>1998.0604393000001</v>
+        <v>120031.5436571</v>
       </c>
       <c r="D13" s="0">
-        <v>2022.0608434000001</v>
+        <v>120055.543983</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>5</v>
@@ -321,13 +321,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0">
-        <v>25.999831900000117</v>
+        <v>25.999850799998967</v>
       </c>
       <c r="C14" s="0">
-        <v>1998.0604369</v>
+        <v>120031.54365610001</v>
       </c>
       <c r="D14" s="0">
-        <v>2024.0612232000001</v>
+        <v>120057.54415440001</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>5</v>
@@ -338,13 +338,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0">
-        <v>27.999381900000117</v>
+        <v>27.99958729998616</v>
       </c>
       <c r="C15" s="0">
-        <v>1998.0604393000001</v>
+        <v>120031.54365719999</v>
       </c>
       <c r="D15" s="0">
-        <v>2026.0607732000001</v>
+        <v>120059.54389089999</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>5</v>
@@ -355,13 +355,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0">
-        <v>30.000027199999977</v>
+        <v>29.999658199987607</v>
       </c>
       <c r="C16" s="0">
-        <v>1998.0604392</v>
+        <v>120031.54365739999</v>
       </c>
       <c r="D16" s="0">
-        <v>2028.0614184999999</v>
+        <v>120061.54396179999</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>5</v>
@@ -372,13 +372,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0">
-        <v>31.999517400000059</v>
+        <v>31.999695299993618</v>
       </c>
       <c r="C17" s="0">
-        <v>1998.0604390000001</v>
+        <v>120031.5436562</v>
       </c>
       <c r="D17" s="0">
-        <v>2030.0609087</v>
+        <v>120063.5439989</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>5</v>
@@ -386,63 +386,71 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0">
-        <v>0</v>
+        <v>33.999601499992423</v>
       </c>
       <c r="C18" s="0">
-        <v>0</v>
+        <v>120031.54365579999</v>
       </c>
       <c r="D18" s="0">
-        <v>0</v>
-      </c>
-      <c r="E18" s="0"/>
+        <v>120065.5439051</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0">
-        <v>0</v>
+        <v>35.999604799988447</v>
       </c>
       <c r="C19" s="0">
-        <v>0</v>
+        <v>120031.5436561</v>
       </c>
       <c r="D19" s="0">
-        <v>0</v>
-      </c>
-      <c r="E19" s="0"/>
+        <v>120067.5439084</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0">
-        <v>0</v>
+        <v>37.999560399999609</v>
       </c>
       <c r="C20" s="0">
-        <v>0</v>
+        <v>120031.54365780001</v>
       </c>
       <c r="D20" s="0">
-        <v>0</v>
-      </c>
-      <c r="E20" s="0"/>
+        <v>120069.54386400001</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0">
-        <v>0</v>
+        <v>39.999620199989295</v>
       </c>
       <c r="C21" s="0">
-        <v>0</v>
+        <v>120031.54365729999</v>
       </c>
       <c r="D21" s="0">
-        <v>0</v>
-      </c>
-      <c r="E21" s="0"/>
+        <v>120071.5439238</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="0">

</xml_diff>